<commit_message>
mcra singlevalue action template
</commit_message>
<xml_diff>
--- a/tasks/mcra/examples/task_input/test_mcra_action_template/Data/SingleValueConsumptions.xlsx
+++ b/tasks/mcra/examples/task_input/test_mcra_action_template/Data/SingleValueConsumptions.xlsx
@@ -1,58 +1,147 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Git/ONTOX/toxindex-task-registry/tasks/mcra/examples/task_input/test_mcra_action_template/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91035990-B365-6645-9306-497458C5A8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Read me" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ConsumptionSingleValues" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Read me" sheetId="1" r:id="rId1"/>
+    <sheet name="ConsumptionSingleValues" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>MCRA Excel dataset template single value consumptions</t>
+  </si>
+  <si>
+    <t>This Excel file is an empty template of an MCRA compliant dataset for single value consumptions. MCRA datasets are composed of one or more relational tables describing the data. Depending on the type of data, some tables may be required and others may be optional. For some types of data, multiple ways of formatting are available, each with way with its own particular requirements. For a detailed description of the data format for single value consumptions, go to:</t>
+  </si>
+  <si>
+    <t>In the Excel format, each data table is specified in a separate sheet. The names of the sheets should comply with the accepted table names of the module(s) for which the data is intended. The table fields must follow the data table formats of the intended modules.</t>
+  </si>
+  <si>
+    <t>You can use this empty template to format own data to upload and use it in MCRA. This can be done by simply adding the data in the worksheets of this document. You can delete the worksheet of the tables that are not needed/required. Also, columns that are not required may be removed from the tables. When ready, the resulting XLSX file can be uploaded to MCRA, which should recognize it as a valid data file containing single value consumptions.</t>
+  </si>
+  <si>
+    <t>For more details on creating and uploading MCRA datasets, and information on other accepted file formats, go to:</t>
+  </si>
+  <si>
+    <t>idPopulation</t>
+  </si>
+  <si>
+    <t>idFood</t>
+  </si>
+  <si>
+    <t>ValueType</t>
+  </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>ConsumptionAmount</t>
+  </si>
+  <si>
+    <t>ConsumptionUnit</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>POP_EU_ADULT_2022</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>Synthetic test</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>gPerKgBWPerDay</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <color rgb="000033CC"/>
       <sz val="11"/>
+      <color rgb="FF0033CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="002F75B5"/>
+        <fgColor rgb="FF2F75B5"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color auto="1"/>
@@ -77,92 +166,35 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,67 +482,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="168" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="168" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>MCRA Excel dataset template single value consumptions</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>This Excel file is an empty template of an MCRA compliant dataset for single value consumptions. MCRA datasets are composed of one or more relational tables describing the data. Depending on the type of data, some tables may be required and others may be optional. For some types of data, multiple ways of formatting are available, each with way with its own particular requirements. For a detailed description of the data format for single value consumptions, go to:</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
+    <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="str">
         <f>HYPERLINK("https://mcra.rivm.nl/documentation/10.2.12/modules/consumption-modules/single-value-consumptions/single-value-consumptions-data-formats.html")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>In the Excel format, each data table is specified in a separate sheet. The names of the sheets should comply with the accepted table names of the module(s) for which the data is intended. The table fields must follow the data table formats of the intended modules.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>You can use this empty template to format own data to upload and use it in MCRA. This can be done by simply adding the data in the worksheets of this document. You can delete the worksheet of the tables that are not needed/required. Also, columns that are not required may be removed from the tables. When ready, the resulting XLSX file can be uploaded to MCRA, which should recognize it as a valid data file containing single value consumptions.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>For more details on creating and uploading MCRA datasets, and information on other accepted file formats, go to:</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3">
+        <v>https://mcra.rivm.nl/documentation/10.2.12/modules/consumption-modules/single-value-consumptions/single-value-consumptions-data-formats.html</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="str">
         <f>HYPERLINK("https://mcra.rivm.nl/documentation/10.2.12/introduction/data-repository/index.html#creating-and-uploading-data-files")</f>
-        <v/>
+        <v>https://mcra.rivm.nl/documentation/10.2.12/introduction/data-repository/index.html#creating-and-uploading-data-files</v>
       </c>
     </row>
   </sheetData>
@@ -519,63 +535,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="16" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="21" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="19" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="13" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>idPopulation</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>idFood</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>ValueType</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Percentile</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>ConsumptionAmount</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>ConsumptionUnit</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1.6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>